<commit_message>
Game Complete, without circle debug drawing
</commit_message>
<xml_diff>
--- a/GameFeatures.xlsx
+++ b/GameFeatures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidu\Desktop\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sidu\Desktop\Final Project\CrudeEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4990E563-72A4-46A6-8D06-98823466CEBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{982ACD35-5B22-4DA3-B9D3-18A6C14013D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{29DDF616-7DE8-442F-A181-D549D679F54E}"/>
   </bookViews>
@@ -84,9 +84,6 @@
     <t xml:space="preserve"> Managers/EventManager.cpp</t>
   </si>
   <si>
-    <t xml:space="preserve"> Managers/Components/Subscription.cpp</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Managers/ObjectFactory.cpp</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t xml:space="preserve"> Managers/PhysicsManager.cpp</t>
   </si>
   <si>
-    <t>Collision resonse</t>
-  </si>
-  <si>
     <t>Maths/Math2d.cpp (Reflections)</t>
   </si>
   <si>
@@ -169,6 +163,12 @@
   </si>
   <si>
     <t>Player loses all hitpoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Components/Subscription.cpp</t>
+  </si>
+  <si>
+    <t>Collision resolution</t>
   </si>
 </sst>
 </file>
@@ -224,6 +224,9 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -241,9 +244,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -258,11 +258,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{458CFAA4-DEC7-4667-AB88-1A8521B66245}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{458CFAA4-DEC7-4667-AB88-1A8521B66245}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:C23" xr:uid="{2F1D7DE2-85BF-40BD-9034-D929972E59DF}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{90BA49A2-E35F-4BA3-B96E-D406388BFD55}" name="Feature"/>
-    <tableColumn id="2" xr3:uid="{E6FDD434-47F7-4FBC-AF17-EEE0CCAF0EE5}" name="Implemented" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{E6FDD434-47F7-4FBC-AF17-EEE0CCAF0EE5}" name="Implemented" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{F788D9D5-9249-4BC6-9D52-17FC7D4DC09F}" name="File Location"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -569,7 +569,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,7 +584,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
@@ -595,7 +595,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -606,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -617,7 +617,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -628,10 +628,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -639,10 +639,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -650,10 +650,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -661,10 +661,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -683,10 +683,10 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -694,10 +694,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -705,10 +705,10 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -716,7 +716,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>16</v>
@@ -724,112 +724,112 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" t="s">
         <v>45</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>